<commit_message>
removed reference to non-existing concept in Zilo
</commit_message>
<xml_diff>
--- a/lists/zilo.xlsx
+++ b/lists/zilo.xlsx
@@ -11,12 +11,12 @@
     <sheet name="lexcauc" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">lexcauc!$B$1:$K$1725</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">lexcauc!$B$1:$AD$1725</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Excel_BuiltIn__FilterDatabase" vbProcedure="false">lexcauc!$I$1:$K$2310</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="parameters" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="parameters_1" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="parameters_2" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">lexcauc!$B$1:$AD$1725</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">lexcauc!$B$1:$K$1725</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -11883,10 +11883,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="K1537" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H1549" activeCellId="0" sqref="H1549"/>
+      <selection pane="bottomLeft" activeCell="D1549" activeCellId="0" sqref="D1549"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.37109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="5.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.15"/>
@@ -51688,7 +51688,7 @@
       </c>
       <c r="C1549" s="1"/>
       <c r="D1549" s="1" t="n">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="F1549" s="2" t="s">
         <v>3281</v>
@@ -56162,7 +56162,7 @@
       <c r="K1728" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:K1725"/>
+  <autoFilter ref="B1:AD1725"/>
   <conditionalFormatting sqref="AE1:IO1 D1:AC1">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(TRIM(D1))&gt;0</formula>

</xml_diff>